<commit_message>
QA ONB test and L1 regression
</commit_message>
<xml_diff>
--- a/Python/Iterations_ numb.xlsx
+++ b/Python/Iterations_ numb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
   <si>
     <t xml:space="preserve">Lp problem </t>
   </si>
@@ -143,15 +143,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I28"/>
+  <dimension ref="A2:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,17 +473,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -960,10 +960,10 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G20">
         <v>7</v>
@@ -1204,6 +1204,35 @@
         <v>8</v>
       </c>
       <c r="I28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>13</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29">
+        <v>8</v>
+      </c>
+      <c r="I29">
         <v>11</v>
       </c>
     </row>
@@ -1220,7 +1249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -1234,16 +1263,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1281,7 +1310,7 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1475,7 +1504,7 @@
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="3">
         <v>6.2857099999999999</v>
       </c>
     </row>
@@ -1489,7 +1518,7 @@
       <c r="C19">
         <v>2</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1520,7 +1549,7 @@
       <c r="C21">
         <v>3</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="3">
         <v>4</v>
       </c>
     </row>
@@ -1534,7 +1563,7 @@
       <c r="C22">
         <v>2</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="3">
         <v>8</v>
       </c>
     </row>
@@ -1605,7 +1634,7 @@
       <c r="C26">
         <v>10</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1619,7 +1648,7 @@
       <c r="C27">
         <v>50</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1633,12 +1662,12 @@
       <c r="C28">
         <v>8</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D29" s="6"/>
+      <c r="D29" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>